<commit_message>
consent and children (#94)
</commit_message>
<xml_diff>
--- a/test_data/ParentalConsent_Doubles.xlsx
+++ b/test_data/ParentalConsent_Doubles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/chinmay_mudholkar1_nhs_net/Documents/VSCode/manage-vaccinations-in-schools-testing/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_29F4BEC59605FFA1F8E8A78AEB924F4CBE121BFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5A1D88-55B2-4DF9-A961-4C8D00DC84FA}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_29F4BEC59605FFA1F8E8A78AEB924F4CBE121BFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86607970-589B-46E2-AA84-7E5214007DF9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>ScenarioID</t>
   </si>
@@ -234,11 +234,14 @@
 EMILIA MADDOX is due to get the MenACWY and Td/IPV vaccinations at school</t>
   </si>
   <si>
-    <t>Consent confirmed
+    <t>Personal choice</t>
+  </si>
+  <si>
+    <t>Consent for the MenACWY vaccination confirmed
 As you answered ‘yes’ to some of the health questions, we need to check the MenACWY vaccination is suitable for ROSE VOSE. We’ll review your answers and get in touch again soon.</t>
   </si>
   <si>
-    <t>Consent confirmed
+    <t>Consent for the Td/IPV vaccination confirmed
 SUSAN BYRON is due to get the Td/IPV vaccination at school on</t>
   </si>
 </sst>
@@ -751,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,10 +1063,14 @@
       </c>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="8"/>
+      <c r="Z4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="AB4" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1124,10 +1131,14 @@
       <c r="W5" s="5"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="8"/>
+      <c r="Z5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="AB5" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>